<commit_message>
Update to electron 12. Update test reference files
</commit_message>
<xml_diff>
--- a/test/refdata/selection_save_multi.xlsx
+++ b/test/refdata/selection_save_multi.xlsx
@@ -10,6 +10,28 @@
     <definedName name="_xlnm._FilterDatabase" localSheetId="1">'specobjects'!A1:E13</definedName>
   </definedNames>
 </workbook>
+</file>
+
+<file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
+<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xlrd="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
+  <metadataTypes count="1">
+    <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
+  </metadataTypes>
+  <futureMetadata name="XLDAPR" count="1">
+    <bk>
+      <extLst>
+        <ext uri="{bdbb8cdc-fa1e-496e-a857-3c3f30c029c3}">
+          <xda:dynamicArrayProperties fDynamic="1" fCollapsed="0"/>
+        </ext>
+      </extLst>
+    </bk>
+  </futureMetadata>
+  <cellMetadata count="1">
+    <bk>
+      <rc t="1" v="0"/>
+    </bk>
+  </cellMetadata>
+</metadata>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>

</xml_diff>